<commit_message>
massa de dados dinamica via excel
</commit_message>
<xml_diff>
--- a/src/test/resources/TDD_AdvantageOnlineShoppingData.xlsx
+++ b/src/test/resources/TDD_AdvantageOnlineShoppingData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\george.junior\git\TDD_AdvantageMobileShopping\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4EFCC26-A6F5-4195-BCF2-22309DB48BDB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69E3E221-1830-4E37-A907-15F659049E7E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="586" firstSheet="2" activeTab="3" xr2:uid="{D4DEB64E-DE7E-45FC-8D49-61962D919F60}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="586" firstSheet="2" activeTab="3" xr2:uid="{D4DEB64E-DE7E-45FC-8D49-61962D919F60}"/>
   </bookViews>
   <sheets>
     <sheet name="AcessarUmProdutoPelaHome_Po" sheetId="1" r:id="rId1"/>
@@ -20,23 +20,17 @@
     <sheet name="BuscarUmProdutoPelaBusca_Po" sheetId="5" r:id="rId5"/>
     <sheet name="BuscarUmProdutoPelaBusca_Ne" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="52">
   <si>
     <t>produto</t>
   </si>
@@ -98,12 +92,6 @@
     <t>Abc123</t>
   </si>
   <si>
-    <t>teste1@teste.com</t>
-  </si>
-  <si>
-    <t>teste1</t>
-  </si>
-  <si>
     <t>da silva</t>
   </si>
   <si>
@@ -167,13 +155,37 @@
     <t>DeveRealisarUmaBuscaDeProdutoInvalido</t>
   </si>
   <si>
-    <t>DeveTentarCadasTrarUmNovoClienteComFalha</t>
-  </si>
-  <si>
     <t>Samsung</t>
   </si>
   <si>
-    <t>autoTeste</t>
+    <t>George</t>
+  </si>
+  <si>
+    <t>Ana</t>
+  </si>
+  <si>
+    <t>GeorgeTester</t>
+  </si>
+  <si>
+    <t>AnaTester</t>
+  </si>
+  <si>
+    <t>PauloTester</t>
+  </si>
+  <si>
+    <t>GeorgeTester@teste.com</t>
+  </si>
+  <si>
+    <t>AnaTester@teste.com</t>
+  </si>
+  <si>
+    <t>PauloTester@teste.com</t>
+  </si>
+  <si>
+    <t>Paulo</t>
+  </si>
+  <si>
+    <t>Japan</t>
   </si>
 </sst>
 </file>
@@ -224,13 +236,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -561,21 +574,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -583,31 +596,31 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>34</v>
+        <v>27</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>35</v>
+        <v>28</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>38</v>
+        <v>29</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -633,13 +646,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -647,39 +660,39 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>38</v>
+      <c r="C6" s="2" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -689,184 +702,186 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47748592-BB78-41A0-8ED8-959B95E0445B}">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection sqref="A1:L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.85546875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="E1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G1" t="s">
+      <c r="F1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H1" t="s">
+      <c r="G1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="I1" t="s">
+      <c r="H1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="J1" t="s">
+      <c r="I1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="K1" t="s">
-        <v>16</v>
-      </c>
-      <c r="L1" t="s">
-        <v>17</v>
-      </c>
-      <c r="M1" t="s">
+      <c r="L1" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="3">
+        <v>989997979</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="L2" s="3">
+        <v>18060605</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B3" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E3" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G3" s="3">
+        <v>989997979</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="L3" s="3">
+        <v>18060605</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="3">
+        <v>989997979</v>
+      </c>
+      <c r="H4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H2">
-        <v>989997979</v>
-      </c>
-      <c r="I2" t="s">
-        <v>23</v>
-      </c>
-      <c r="J2" t="s">
-        <v>24</v>
-      </c>
-      <c r="K2" t="s">
-        <v>25</v>
-      </c>
-      <c r="L2" t="s">
-        <v>26</v>
-      </c>
-      <c r="M2">
-        <v>18060605</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H3">
-        <v>989997979</v>
-      </c>
-      <c r="I3" t="s">
-        <v>23</v>
-      </c>
-      <c r="J3" t="s">
-        <v>24</v>
-      </c>
-      <c r="K3" t="s">
-        <v>25</v>
-      </c>
-      <c r="L3" t="s">
-        <v>26</v>
-      </c>
-      <c r="M3">
-        <v>18060605</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" t="s">
-        <v>21</v>
-      </c>
-      <c r="G4" t="s">
-        <v>22</v>
-      </c>
-      <c r="H4">
-        <v>989997979</v>
-      </c>
-      <c r="I4" t="s">
-        <v>23</v>
-      </c>
-      <c r="J4" t="s">
-        <v>24</v>
-      </c>
-      <c r="K4" t="s">
-        <v>25</v>
-      </c>
-      <c r="L4" t="s">
-        <v>26</v>
-      </c>
-      <c r="M4">
+      <c r="L4" s="3">
         <v>18060605</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{08D936AE-3017-420E-A5FB-7C99FAFD8BE4}"/>
-    <hyperlink ref="E3" r:id="rId2" xr:uid="{7BE67FB5-D6A1-477E-BF9B-15EA0A912C3F}"/>
-    <hyperlink ref="E4" r:id="rId3" xr:uid="{F22FB943-933C-401B-A761-0F16DA00C3AA}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{54449EBE-9801-4398-937D-5DFFB357730B}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{02188FC2-4DDA-4637-836F-2224699D6C6B}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{A7BF6B7D-3DE2-4C65-9458-852D05B48827}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
@@ -875,186 +890,184 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0A2C4E6-CCD4-41FE-AB5C-3F2F51B1DE80}">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="12.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" style="3" customWidth="1"/>
+    <col min="4" max="4" width="8.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="8.85546875" style="3"/>
+    <col min="13" max="13" width="9.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.85546875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="3">
+        <v>989997979</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="L2" s="3">
+        <v>18060605</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J1" t="s">
-        <v>15</v>
-      </c>
-      <c r="K1" t="s">
-        <v>16</v>
-      </c>
-      <c r="L1" t="s">
-        <v>17</v>
-      </c>
-      <c r="M1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="F3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="3">
+        <v>989997979</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="L3" s="3">
+        <v>18060605</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E4" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G4" s="3">
+        <v>989997979</v>
+      </c>
+      <c r="H4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H2">
-        <v>989997979</v>
-      </c>
-      <c r="I2" t="s">
-        <v>23</v>
-      </c>
-      <c r="J2" t="s">
-        <v>24</v>
-      </c>
-      <c r="K2" t="s">
-        <v>25</v>
-      </c>
-      <c r="L2" t="s">
-        <v>26</v>
-      </c>
-      <c r="M2">
-        <v>18060605</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H3">
-        <v>989997979</v>
-      </c>
-      <c r="I3" t="s">
-        <v>23</v>
-      </c>
-      <c r="J3" t="s">
-        <v>24</v>
-      </c>
-      <c r="K3" t="s">
-        <v>25</v>
-      </c>
-      <c r="L3" t="s">
-        <v>26</v>
-      </c>
-      <c r="M3">
-        <v>18060605</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" t="s">
-        <v>21</v>
-      </c>
-      <c r="G4" t="s">
-        <v>22</v>
-      </c>
-      <c r="H4">
-        <v>989997979</v>
-      </c>
-      <c r="I4" t="s">
-        <v>23</v>
-      </c>
-      <c r="J4" t="s">
-        <v>24</v>
-      </c>
-      <c r="K4" t="s">
-        <v>25</v>
-      </c>
-      <c r="L4" t="s">
-        <v>26</v>
-      </c>
-      <c r="M4">
+      <c r="L4" s="3">
         <v>18060605</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{2F4CF434-4928-472C-A45E-A687B9060E04}"/>
-    <hyperlink ref="E3" r:id="rId2" xr:uid="{24419471-4843-4B96-B5A2-9D74ABF59607}"/>
-    <hyperlink ref="E4" r:id="rId3" xr:uid="{078ED41D-26D8-43FD-B40F-97DEB41719AB}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{78570A2C-3322-4B0D-90E6-0734652D4FE5}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{EBA9E605-0D39-47E3-B245-359D37A3D44A}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{F783687E-176B-483C-8065-B82CEAA64C7C}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -1116,24 +1129,24 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B3" s="2" t="s">
-        <v>44</v>
+      <c r="B3" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Termino com massa dinamica em todos os casos de teste.
</commit_message>
<xml_diff>
--- a/src/test/resources/TDD_AdvantageOnlineShoppingData.xlsx
+++ b/src/test/resources/TDD_AdvantageOnlineShoppingData.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\george.junior\git\TDD_AdvantageMobileShopping\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69E3E221-1830-4E37-A907-15F659049E7E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9BAF3CB-3610-4429-92AF-09FBAC56AF4F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="586" firstSheet="2" activeTab="3" xr2:uid="{D4DEB64E-DE7E-45FC-8D49-61962D919F60}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="21840" windowHeight="13140" tabRatio="586" firstSheet="3" activeTab="4" xr2:uid="{D4DEB64E-DE7E-45FC-8D49-61962D919F60}"/>
   </bookViews>
   <sheets>
-    <sheet name="AcessarUmProdutoPelaHome_Po" sheetId="1" r:id="rId1"/>
-    <sheet name="AcessarUmProdutoPelaHome_Ne" sheetId="7" r:id="rId2"/>
+    <sheet name="AbrirUmProdutoPelaHome_Po" sheetId="1" r:id="rId1"/>
+    <sheet name="AbrirUmProdutoPelaHome_Ne" sheetId="7" r:id="rId2"/>
     <sheet name="CadastrarNovoCliente_Po" sheetId="3" r:id="rId3"/>
     <sheet name="CadastrarNovoCliente_Ne" sheetId="4" r:id="rId4"/>
     <sheet name="BuscarUmProdutoPelaBusca_Po" sheetId="5" r:id="rId5"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="51">
   <si>
     <t>produto</t>
   </si>
@@ -38,9 +38,6 @@
     <t>HP Stream - 11-d020nr Laptop</t>
   </si>
   <si>
-    <t>DeveRealisarUmaBuscaComSucesso</t>
-  </si>
-  <si>
     <t>HP ELITE X2 1011 G1 TABLET</t>
   </si>
   <si>
@@ -122,12 +119,6 @@
     <t>Logitech G502 Proteus Core</t>
   </si>
   <si>
-    <t>Kensington Orbit 72352 Trackball</t>
-  </si>
-  <si>
-    <t>Ipad</t>
-  </si>
-  <si>
     <t>SPEAKERS</t>
   </si>
   <si>
@@ -146,15 +137,6 @@
     <t>Categoria</t>
   </si>
   <si>
-    <t>deveTentarAbrirPaginaDeUmProdutoInesistentePelaCategoria</t>
-  </si>
-  <si>
-    <t>deveAbrirPaginaDeUmProdutoPelaCategoria</t>
-  </si>
-  <si>
-    <t>DeveRealisarUmaBuscaDeProdutoInvalido</t>
-  </si>
-  <si>
     <t>Samsung</t>
   </si>
   <si>
@@ -186,6 +168,21 @@
   </si>
   <si>
     <t>Japan</t>
+  </si>
+  <si>
+    <t>HP Pavilion 15t Touch Laptop</t>
+  </si>
+  <si>
+    <t>BEATS STUDIO 2 OVER-EAR MATTE BLACK HEADPHONES</t>
+  </si>
+  <si>
+    <t>Bose SoundLink Wireless Speaker</t>
+  </si>
+  <si>
+    <t>HP ElitePad 1000 G2 Tablet</t>
+  </si>
+  <si>
+    <t>HP Z8000 Bluetooth Mouse</t>
   </si>
 </sst>
 </file>
@@ -559,68 +556,65 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80702A83-724E-4768-B1BE-90F73797AA16}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection sqref="A1:A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="53" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>31</v>
+      </c>
       <c r="B2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>32</v>
+      </c>
       <c r="B3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="B4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" t="s">
         <v>28</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -631,68 +625,65 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B404657F-C05F-2A44-AAD2-7863EF0C7397}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="57.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="33.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>31</v>
+      </c>
       <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>32</v>
+      </c>
       <c r="B3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="B4" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C5" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -727,75 +718,75 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="D1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="J1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>17</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>19</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>20</v>
       </c>
       <c r="G2" s="3">
         <v>989997979</v>
       </c>
       <c r="H2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="K2" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>22</v>
       </c>
       <c r="L2" s="3">
         <v>18060605</v>
@@ -803,37 +794,37 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>19</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>20</v>
       </c>
       <c r="G3" s="3">
         <v>989997979</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="I3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J3" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="J3" s="3" t="s">
-        <v>24</v>
-      </c>
       <c r="K3" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L3" s="3">
         <v>18060605</v>
@@ -841,37 +832,37 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>19</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>20</v>
       </c>
       <c r="G4" s="3">
         <v>989997979</v>
       </c>
       <c r="H4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="K4" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>22</v>
       </c>
       <c r="L4" s="3">
         <v>18060605</v>
@@ -892,7 +883,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0A2C4E6-CCD4-41FE-AB5C-3F2F51B1DE80}">
   <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -913,75 +904,75 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="D1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="J1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>17</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>19</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>20</v>
       </c>
       <c r="G2" s="3">
         <v>989997979</v>
       </c>
       <c r="H2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="K2" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>22</v>
       </c>
       <c r="L2" s="3">
         <v>18060605</v>
@@ -989,37 +980,37 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>19</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>20</v>
       </c>
       <c r="G3" s="3">
         <v>989997979</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="I3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J3" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="J3" s="3" t="s">
-        <v>24</v>
-      </c>
       <c r="K3" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L3" s="3">
         <v>18060605</v>
@@ -1027,37 +1018,37 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>19</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>20</v>
       </c>
       <c r="G4" s="3">
         <v>989997979</v>
       </c>
       <c r="H4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="K4" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>22</v>
       </c>
       <c r="L4" s="3">
         <v>18060605</v>
@@ -1075,37 +1066,35 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91BC3573-0780-4934-A8A2-22FE942CCBF3}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="53.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="53.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -1115,39 +1104,35 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBC9FEAF-7142-4F95-BC1C-879216998CD6}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection sqref="A1:A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B3" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B4" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>